<commit_message>
add Selenium IDE test suite
</commit_message>
<xml_diff>
--- a/ManualTestCase.xlsx
+++ b/ManualTestCase.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="0" windowWidth="25120" windowHeight="15540" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14620" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -12,7 +12,7 @@
   <externalReferences>
     <externalReference r:id="rId2"/>
   </externalReferences>
-  <calcPr calcId="140000" concurrentCalc="0"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="298" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="336" uniqueCount="114">
   <si>
     <t>Environment</t>
   </si>
@@ -102,9 +102,6 @@
     <t>Attach any file with unsupported format (e.g. test.gif)</t>
   </si>
   <si>
-    <t>Start typing an existing recipient address/name (e.g. JOOR)</t>
-  </si>
-  <si>
     <t>Send a Message - Send to all my Connections</t>
   </si>
   <si>
@@ -165,9 +162,6 @@
       </rPr>
       <t xml:space="preserve"> tab from the Header tool bar</t>
     </r>
-  </si>
-  <si>
-    <t>The autocomplete pop up with filtered addresses/names appears</t>
   </si>
   <si>
     <t xml:space="preserve">Navigate to the https://staging.joordev.com/ 
@@ -1100,9 +1094,6 @@
     <t>Send a Message - Select Connection (more than 1 recipients)</t>
   </si>
   <si>
-    <t>Start typing an existing recipients address/name (e.g. JOOR, JOOR FLORIDA, etc.)</t>
-  </si>
-  <si>
     <t>Recipient addresses appear in the recipient input</t>
   </si>
   <si>
@@ -1144,9 +1135,6 @@
     <t>Previous recipient selections are closed</t>
   </si>
   <si>
-    <t>Send a Message - Recipient Selection</t>
-  </si>
-  <si>
     <r>
       <t xml:space="preserve">Verify the </t>
     </r>
@@ -1257,6 +1245,70 @@
       </rPr>
       <t xml:space="preserve"> pop up by clicking X in the upper right corner of the page</t>
     </r>
+  </si>
+  <si>
+    <t>Verify pop up message after sending message</t>
+  </si>
+  <si>
+    <t>Pop up with message "Your message has been sent" appears</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Pop up with message </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t>"Your message has been sent</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t>" appears</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Pop up with message "</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t>Your message has been sent</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t>" appears</t>
+    </r>
+  </si>
+  <si>
+    <t>Send a Message - Select and Clear Recipient name/address</t>
+  </si>
+  <si>
+    <t>Start typing an existing recipients names/addresses (e.g. JOOR, JOOR FLORIDA, etc.)</t>
+  </si>
+  <si>
+    <t>The autocomplete pop up with filtered names/addresses appears</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Choose the existing recipient name/address from the autocomplete pop up </t>
+  </si>
+  <si>
+    <t>Start typing an existing recipient name/address (e.g. JOOR)</t>
+  </si>
+  <si>
+    <t>The autocomplete pop up with filtered name/address appears</t>
   </si>
 </sst>
 </file>
@@ -1348,7 +1400,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -1371,8 +1423,21 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="251">
+  <cellStyleXfs count="259">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1624,8 +1689,16 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1689,8 +1762,14 @@
     <xf numFmtId="14" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="251">
+  <cellStyles count="259">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -1816,6 +1895,10 @@
     <cellStyle name="Followed Hyperlink" xfId="246" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="248" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="250" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="252" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="254" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="256" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="258" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -1941,9 +2024,274 @@
     <cellStyle name="Hyperlink" xfId="245" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="247" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="249" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="251" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="253" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="255" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="257" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="15">
+  <dxfs count="30">
+    <dxf>
+      <font>
+        <b/>
+        <color rgb="FFD53333"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFFFFF"/>
+          <bgColor rgb="FFFFFFFF"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <color rgb="FF0ECB0B"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFFFFF"/>
+          <bgColor rgb="FFFFFFFF"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFFFFFF"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFA61C00"/>
+          <bgColor rgb="FFA61C00"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFFFFFF"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFF0000"/>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFFFFFF"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF38761D"/>
+          <bgColor rgb="FF38761D"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <color rgb="FFD53333"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFFFFF"/>
+          <bgColor rgb="FFFFFFFF"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <color rgb="FF0ECB0B"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFFFFF"/>
+          <bgColor rgb="FFFFFFFF"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFFFFFF"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFA61C00"/>
+          <bgColor rgb="FFA61C00"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFFFFFF"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFF0000"/>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFFFFFF"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF38761D"/>
+          <bgColor rgb="FF38761D"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <color rgb="FFD53333"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFFFFF"/>
+          <bgColor rgb="FFFFFFFF"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <color rgb="FF0ECB0B"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFFFFF"/>
+          <bgColor rgb="FFFFFFFF"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFFFFFF"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFA61C00"/>
+          <bgColor rgb="FFA61C00"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFFFFFF"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFF0000"/>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFFFFFF"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF38761D"/>
+          <bgColor rgb="FF38761D"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
     <dxf>
       <font>
         <b/>
@@ -2605,10 +2953,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:I686"/>
+  <dimension ref="A2:I691"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="D98" sqref="D98"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0"/>
@@ -2626,16 +2974,16 @@
   <sheetData>
     <row r="2" spans="1:9" ht="24">
       <c r="A2" s="8" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="C2" s="8"/>
     </row>
     <row r="3" spans="1:9">
       <c r="A3" s="8" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="B3" s="22">
         <v>42775</v>
@@ -2644,7 +2992,7 @@
     </row>
     <row r="4" spans="1:9">
       <c r="A4" s="8" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B4" s="19">
         <v>1</v>
@@ -2662,7 +3010,7 @@
         <v>2</v>
       </c>
       <c r="D5" s="21" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="E5" s="21" t="s">
         <v>3</v>
@@ -2688,7 +3036,7 @@
         <v>1</v>
       </c>
       <c r="C6" s="9" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="D6" s="10" t="s">
         <v>10</v>
@@ -2707,7 +3055,7 @@
       <c r="C7" s="6"/>
       <c r="D7" s="6"/>
       <c r="E7" s="6" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="F7" s="7" t="s">
         <v>14</v>
@@ -2744,10 +3092,10 @@
         <v>2</v>
       </c>
       <c r="C9" s="9" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D9" s="10" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="E9" s="6"/>
       <c r="F9" s="7"/>
@@ -2764,10 +3112,10 @@
       <c r="C10" s="6"/>
       <c r="D10" s="6"/>
       <c r="E10" s="6" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F10" s="7" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="G10" s="6"/>
       <c r="H10" s="7"/>
@@ -2784,10 +3132,10 @@
       <c r="C11" s="6"/>
       <c r="D11" s="6"/>
       <c r="E11" s="6" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="F11" s="6" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="G11" s="6"/>
       <c r="H11" s="4"/>
@@ -2804,10 +3152,10 @@
       <c r="C12" s="6"/>
       <c r="D12" s="6"/>
       <c r="E12" s="6" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="F12" s="6" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="G12" s="6"/>
       <c r="H12" s="4"/>
@@ -2824,13 +3172,13 @@
       <c r="C13" s="6"/>
       <c r="D13" s="6"/>
       <c r="E13" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="F13" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="G13" s="6" t="s">
         <v>56</v>
-      </c>
-      <c r="F13" s="6" t="s">
-        <v>54</v>
-      </c>
-      <c r="G13" s="6" t="s">
-        <v>58</v>
       </c>
       <c r="H13" s="4"/>
       <c r="I13" s="11" t="s">
@@ -2846,10 +3194,10 @@
       <c r="C14" s="6"/>
       <c r="D14" s="6"/>
       <c r="E14" s="6" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="F14" s="6" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="G14" s="6"/>
       <c r="H14" s="4"/>
@@ -2863,10 +3211,10 @@
         <v>3</v>
       </c>
       <c r="C15" s="9" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D15" s="10" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E15" s="6"/>
       <c r="F15" s="6"/>
@@ -2882,14 +3230,16 @@
       <c r="C16" s="6"/>
       <c r="D16" s="6"/>
       <c r="E16" s="6" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F16" s="6" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="G16" s="6"/>
       <c r="H16" s="4"/>
-      <c r="I16" s="11"/>
+      <c r="I16" s="11" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="17" spans="1:9" ht="34" customHeight="1">
       <c r="A17" s="12"/>
@@ -2899,14 +3249,16 @@
       <c r="C17" s="6"/>
       <c r="D17" s="6"/>
       <c r="E17" s="6" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="F17" s="6" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="G17" s="6"/>
       <c r="H17" s="4"/>
-      <c r="I17" s="11"/>
+      <c r="I17" s="11" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="18" spans="1:9" ht="34" customHeight="1">
       <c r="A18" s="12"/>
@@ -2916,14 +3268,16 @@
       <c r="C18" s="6"/>
       <c r="D18" s="6"/>
       <c r="E18" s="6" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="F18" s="14" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="G18" s="6"/>
       <c r="H18" s="4"/>
-      <c r="I18" s="11"/>
+      <c r="I18" s="11" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="19" spans="1:9" ht="50" customHeight="1">
       <c r="A19" s="12"/>
@@ -2933,14 +3287,16 @@
       <c r="C19" s="6"/>
       <c r="D19" s="6"/>
       <c r="E19" s="6" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="F19" s="6" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="G19" s="6"/>
       <c r="H19" s="4"/>
-      <c r="I19" s="11"/>
+      <c r="I19" s="11" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="20" spans="1:9" ht="34" customHeight="1">
       <c r="A20" s="12"/>
@@ -2948,10 +3304,10 @@
         <v>4</v>
       </c>
       <c r="C20" s="9" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D20" s="10" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="E20" s="6"/>
       <c r="F20" s="6"/>
@@ -2967,14 +3323,16 @@
       <c r="C21" s="6"/>
       <c r="D21" s="6"/>
       <c r="E21" s="6" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F21" s="6" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="G21" s="6"/>
       <c r="H21" s="4"/>
-      <c r="I21" s="11"/>
+      <c r="I21" s="24" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="22" spans="1:9" ht="34" customHeight="1">
       <c r="A22" s="12"/>
@@ -2984,14 +3342,16 @@
       <c r="C22" s="6"/>
       <c r="D22" s="6"/>
       <c r="E22" s="6" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="F22" s="6" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="G22" s="6"/>
       <c r="H22" s="4"/>
-      <c r="I22" s="11"/>
+      <c r="I22" s="24" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="23" spans="1:9" ht="34" customHeight="1">
       <c r="A23" s="12"/>
@@ -3001,14 +3361,16 @@
       <c r="C23" s="6"/>
       <c r="D23" s="6"/>
       <c r="E23" s="6" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="F23" s="6" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="G23" s="6"/>
       <c r="H23" s="4"/>
-      <c r="I23" s="11"/>
+      <c r="I23" s="24" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="24" spans="1:9" ht="34" customHeight="1">
       <c r="A24" s="12"/>
@@ -3018,14 +3380,16 @@
       <c r="C24" s="6"/>
       <c r="D24" s="6"/>
       <c r="E24" s="6" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="F24" s="6" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="G24" s="6"/>
       <c r="H24" s="4"/>
-      <c r="I24" s="11"/>
+      <c r="I24" s="24" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="25" spans="1:9" ht="46" customHeight="1">
       <c r="A25" s="12"/>
@@ -3035,14 +3399,16 @@
       <c r="C25" s="6"/>
       <c r="D25" s="6"/>
       <c r="E25" s="6" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="F25" s="6" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="G25" s="6"/>
       <c r="H25" s="4"/>
-      <c r="I25" s="11"/>
+      <c r="I25" s="24" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="26" spans="1:9" ht="48">
       <c r="A26" s="12"/>
@@ -3050,10 +3416,10 @@
         <v>5</v>
       </c>
       <c r="C26" s="9" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="D26" s="10" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E26" s="6"/>
       <c r="F26" s="6"/>
@@ -3069,10 +3435,10 @@
       <c r="C27" s="6"/>
       <c r="D27" s="13"/>
       <c r="E27" s="6" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="F27" s="6" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="G27" s="6"/>
       <c r="H27" s="4"/>
@@ -3088,10 +3454,10 @@
       <c r="C28" s="6"/>
       <c r="D28" s="4"/>
       <c r="E28" s="6" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="F28" s="14" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="G28" s="6"/>
       <c r="H28" s="4"/>
@@ -3107,10 +3473,10 @@
       <c r="C29" s="6"/>
       <c r="D29" s="6"/>
       <c r="E29" s="6" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="F29" s="6" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="G29" s="4"/>
       <c r="H29" s="4"/>
@@ -3126,10 +3492,10 @@
       <c r="C30" s="6"/>
       <c r="D30" s="6"/>
       <c r="E30" s="6" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="F30" s="6" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="G30" s="4"/>
       <c r="H30" s="4"/>
@@ -3143,10 +3509,10 @@
         <v>6</v>
       </c>
       <c r="C31" s="9" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="D31" s="10" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E31" s="4"/>
       <c r="F31" s="4"/>
@@ -3162,10 +3528,10 @@
       <c r="C32" s="15"/>
       <c r="D32" s="13"/>
       <c r="E32" s="6" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="F32" s="6" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="G32" s="4"/>
       <c r="H32" s="4"/>
@@ -3181,10 +3547,10 @@
       <c r="C33" s="15"/>
       <c r="D33" s="13"/>
       <c r="E33" s="6" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="F33" s="14" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="G33" s="4"/>
       <c r="H33" s="4"/>
@@ -3200,10 +3566,10 @@
       <c r="C34" s="6"/>
       <c r="D34" s="6"/>
       <c r="E34" s="6" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="F34" s="6" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="G34" s="4"/>
       <c r="H34" s="4"/>
@@ -3219,10 +3585,10 @@
       <c r="C35" s="6"/>
       <c r="D35" s="6"/>
       <c r="E35" s="6" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="F35" s="6" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="G35" s="4"/>
       <c r="H35" s="4"/>
@@ -3236,10 +3602,10 @@
         <v>7</v>
       </c>
       <c r="C36" s="9" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="D36" s="10" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E36" s="6"/>
       <c r="F36" s="6"/>
@@ -3255,10 +3621,10 @@
       <c r="C37" s="6"/>
       <c r="D37" s="6"/>
       <c r="E37" s="6" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="F37" s="6" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="G37" s="4"/>
       <c r="H37" s="4"/>
@@ -3274,10 +3640,10 @@
       <c r="C38" s="6"/>
       <c r="D38" s="6"/>
       <c r="E38" s="6" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="F38" s="14" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="G38" s="4"/>
       <c r="H38" s="4"/>
@@ -3293,10 +3659,10 @@
       <c r="C39" s="6"/>
       <c r="D39" s="6"/>
       <c r="E39" s="6" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="F39" s="6" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="G39" s="4"/>
       <c r="H39" s="4"/>
@@ -3312,10 +3678,10 @@
       <c r="C40" s="6"/>
       <c r="D40" s="6"/>
       <c r="E40" s="6" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="F40" s="6" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="G40" s="4"/>
       <c r="H40" s="4"/>
@@ -3331,10 +3697,10 @@
       <c r="C41" s="6"/>
       <c r="D41" s="6"/>
       <c r="E41" s="6" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="F41" s="6" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="G41" s="4"/>
       <c r="H41" s="4"/>
@@ -3342,54 +3708,54 @@
         <v>8</v>
       </c>
     </row>
-    <row r="42" spans="1:9" ht="48">
+    <row r="42" spans="1:9" ht="24">
       <c r="A42" s="12"/>
       <c r="B42" s="19">
-        <v>8</v>
-      </c>
-      <c r="C42" s="9" t="s">
-        <v>45</v>
-      </c>
-      <c r="D42" s="10" t="s">
-        <v>29</v>
-      </c>
-      <c r="E42" s="6"/>
-      <c r="F42" s="6"/>
+        <v>7.6</v>
+      </c>
+      <c r="C42" s="6"/>
+      <c r="D42" s="6"/>
+      <c r="E42" s="6" t="s">
+        <v>104</v>
+      </c>
+      <c r="F42" s="6" t="s">
+        <v>106</v>
+      </c>
       <c r="G42" s="4"/>
       <c r="H42" s="4"/>
-      <c r="I42" s="4"/>
-    </row>
-    <row r="43" spans="1:9" ht="24">
+      <c r="I42" s="16" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" ht="48">
       <c r="A43" s="12"/>
       <c r="B43" s="19">
-        <v>8.1</v>
-      </c>
-      <c r="C43" s="15"/>
-      <c r="D43" s="13"/>
-      <c r="E43" s="6" t="s">
-        <v>68</v>
-      </c>
-      <c r="F43" s="6" t="s">
-        <v>54</v>
-      </c>
+        <v>8</v>
+      </c>
+      <c r="C43" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="D43" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="E43" s="6"/>
+      <c r="F43" s="6"/>
       <c r="G43" s="4"/>
       <c r="H43" s="4"/>
-      <c r="I43" s="16" t="s">
-        <v>8</v>
-      </c>
+      <c r="I43" s="4"/>
     </row>
     <row r="44" spans="1:9" ht="24">
       <c r="A44" s="12"/>
       <c r="B44" s="19">
-        <v>8.1999999999999993</v>
+        <v>8.1</v>
       </c>
       <c r="C44" s="15"/>
       <c r="D44" s="13"/>
       <c r="E44" s="6" t="s">
-        <v>60</v>
-      </c>
-      <c r="F44" s="14" t="s">
-        <v>61</v>
+        <v>66</v>
+      </c>
+      <c r="F44" s="6" t="s">
+        <v>52</v>
       </c>
       <c r="G44" s="4"/>
       <c r="H44" s="4"/>
@@ -3400,15 +3766,15 @@
     <row r="45" spans="1:9" ht="24">
       <c r="A45" s="12"/>
       <c r="B45" s="19">
-        <v>8.3000000000000007</v>
+        <v>8.1999999999999993</v>
       </c>
       <c r="C45" s="15"/>
       <c r="D45" s="13"/>
       <c r="E45" s="6" t="s">
-        <v>62</v>
-      </c>
-      <c r="F45" s="6" t="s">
-        <v>63</v>
+        <v>58</v>
+      </c>
+      <c r="F45" s="14" t="s">
+        <v>59</v>
       </c>
       <c r="G45" s="4"/>
       <c r="H45" s="4"/>
@@ -3419,15 +3785,15 @@
     <row r="46" spans="1:9" ht="24">
       <c r="A46" s="12"/>
       <c r="B46" s="19">
-        <v>8.4</v>
+        <v>8.3000000000000007</v>
       </c>
       <c r="C46" s="15"/>
       <c r="D46" s="13"/>
       <c r="E46" s="6" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="F46" s="6" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="G46" s="4"/>
       <c r="H46" s="4"/>
@@ -3438,15 +3804,15 @@
     <row r="47" spans="1:9" ht="24">
       <c r="A47" s="12"/>
       <c r="B47" s="19">
-        <v>8.5</v>
-      </c>
-      <c r="C47" s="6"/>
-      <c r="D47" s="6"/>
+        <v>8.4</v>
+      </c>
+      <c r="C47" s="15"/>
+      <c r="D47" s="13"/>
       <c r="E47" s="6" t="s">
-        <v>15</v>
+        <v>62</v>
       </c>
       <c r="F47" s="6" t="s">
-        <v>28</v>
+        <v>63</v>
       </c>
       <c r="G47" s="4"/>
       <c r="H47" s="4"/>
@@ -3454,18 +3820,18 @@
         <v>8</v>
       </c>
     </row>
-    <row r="48" spans="1:9" ht="36">
+    <row r="48" spans="1:9" ht="24">
       <c r="A48" s="12"/>
       <c r="B48" s="19">
-        <v>8.6</v>
+        <v>8.5</v>
       </c>
       <c r="C48" s="6"/>
       <c r="D48" s="6"/>
       <c r="E48" s="6" t="s">
-        <v>66</v>
+        <v>15</v>
       </c>
       <c r="F48" s="6" t="s">
-        <v>71</v>
+        <v>27</v>
       </c>
       <c r="G48" s="4"/>
       <c r="H48" s="4"/>
@@ -3473,35 +3839,37 @@
         <v>8</v>
       </c>
     </row>
-    <row r="49" spans="1:9" ht="48">
+    <row r="49" spans="1:9" ht="36">
       <c r="A49" s="12"/>
       <c r="B49" s="19">
-        <v>9</v>
-      </c>
-      <c r="C49" s="9" t="s">
-        <v>44</v>
-      </c>
-      <c r="D49" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="E49" s="6"/>
-      <c r="F49" s="6"/>
+        <v>8.6</v>
+      </c>
+      <c r="C49" s="6"/>
+      <c r="D49" s="6"/>
+      <c r="E49" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="F49" s="6" t="s">
+        <v>69</v>
+      </c>
       <c r="G49" s="4"/>
       <c r="H49" s="4"/>
-      <c r="I49" s="4"/>
+      <c r="I49" s="16" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="50" spans="1:9" ht="24">
       <c r="A50" s="12"/>
       <c r="B50" s="19">
-        <v>9.1</v>
+        <v>8.6999999999999993</v>
       </c>
       <c r="C50" s="6"/>
       <c r="D50" s="6"/>
       <c r="E50" s="6" t="s">
-        <v>53</v>
+        <v>104</v>
       </c>
       <c r="F50" s="6" t="s">
-        <v>54</v>
+        <v>106</v>
       </c>
       <c r="G50" s="4"/>
       <c r="H50" s="4"/>
@@ -3509,37 +3877,35 @@
         <v>8</v>
       </c>
     </row>
-    <row r="51" spans="1:9" ht="24">
+    <row r="51" spans="1:9" ht="48">
       <c r="A51" s="12"/>
       <c r="B51" s="19">
-        <v>9.1999999999999993</v>
-      </c>
-      <c r="C51" s="6"/>
-      <c r="D51" s="6"/>
-      <c r="E51" s="6" t="s">
-        <v>72</v>
-      </c>
-      <c r="F51" s="14" t="s">
-        <v>61</v>
-      </c>
+        <v>9</v>
+      </c>
+      <c r="C51" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="D51" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="E51" s="6"/>
+      <c r="F51" s="6"/>
       <c r="G51" s="4"/>
       <c r="H51" s="4"/>
-      <c r="I51" s="16" t="s">
-        <v>8</v>
-      </c>
+      <c r="I51" s="4"/>
     </row>
     <row r="52" spans="1:9" ht="24">
       <c r="A52" s="12"/>
       <c r="B52" s="19">
-        <v>9.3000000000000007</v>
+        <v>9.1</v>
       </c>
       <c r="C52" s="6"/>
       <c r="D52" s="6"/>
       <c r="E52" s="6" t="s">
-        <v>62</v>
+        <v>51</v>
       </c>
       <c r="F52" s="6" t="s">
-        <v>63</v>
+        <v>52</v>
       </c>
       <c r="G52" s="4"/>
       <c r="H52" s="4"/>
@@ -3550,15 +3916,15 @@
     <row r="53" spans="1:9" ht="24">
       <c r="A53" s="12"/>
       <c r="B53" s="19">
-        <v>9.4</v>
+        <v>9.1999999999999993</v>
       </c>
       <c r="C53" s="6"/>
       <c r="D53" s="6"/>
       <c r="E53" s="6" t="s">
-        <v>64</v>
-      </c>
-      <c r="F53" s="6" t="s">
-        <v>65</v>
+        <v>70</v>
+      </c>
+      <c r="F53" s="14" t="s">
+        <v>59</v>
       </c>
       <c r="G53" s="4"/>
       <c r="H53" s="4"/>
@@ -3569,15 +3935,15 @@
     <row r="54" spans="1:9" ht="24">
       <c r="A54" s="12"/>
       <c r="B54" s="19">
-        <v>9.5</v>
+        <v>9.3000000000000007</v>
       </c>
       <c r="C54" s="6"/>
       <c r="D54" s="6"/>
       <c r="E54" s="6" t="s">
-        <v>16</v>
+        <v>60</v>
       </c>
       <c r="F54" s="6" t="s">
-        <v>31</v>
+        <v>61</v>
       </c>
       <c r="G54" s="4"/>
       <c r="H54" s="4"/>
@@ -3585,18 +3951,18 @@
         <v>8</v>
       </c>
     </row>
-    <row r="55" spans="1:9" ht="36">
+    <row r="55" spans="1:9" ht="24">
       <c r="A55" s="12"/>
       <c r="B55" s="19">
-        <v>9.6</v>
+        <v>9.4</v>
       </c>
       <c r="C55" s="6"/>
       <c r="D55" s="6"/>
       <c r="E55" s="6" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="F55" s="6" t="s">
-        <v>71</v>
+        <v>63</v>
       </c>
       <c r="G55" s="4"/>
       <c r="H55" s="4"/>
@@ -3604,35 +3970,37 @@
         <v>8</v>
       </c>
     </row>
-    <row r="56" spans="1:9" ht="48">
+    <row r="56" spans="1:9" ht="24">
       <c r="A56" s="12"/>
       <c r="B56" s="19">
-        <v>10</v>
-      </c>
-      <c r="C56" s="9" t="s">
-        <v>45</v>
-      </c>
-      <c r="D56" s="10" t="s">
-        <v>46</v>
-      </c>
-      <c r="E56" s="6"/>
-      <c r="F56" s="6"/>
+        <v>9.5</v>
+      </c>
+      <c r="C56" s="6"/>
+      <c r="D56" s="6"/>
+      <c r="E56" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="F56" s="6" t="s">
+        <v>30</v>
+      </c>
       <c r="G56" s="4"/>
       <c r="H56" s="4"/>
-      <c r="I56" s="4"/>
-    </row>
-    <row r="57" spans="1:9" ht="24">
+      <c r="I56" s="16" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="57" spans="1:9" ht="36">
       <c r="A57" s="12"/>
       <c r="B57" s="19">
-        <v>10.1</v>
+        <v>9.6</v>
       </c>
       <c r="C57" s="6"/>
       <c r="D57" s="6"/>
       <c r="E57" s="6" t="s">
-        <v>53</v>
+        <v>64</v>
       </c>
       <c r="F57" s="6" t="s">
-        <v>54</v>
+        <v>69</v>
       </c>
       <c r="G57" s="4"/>
       <c r="H57" s="4"/>
@@ -3643,15 +4011,15 @@
     <row r="58" spans="1:9" ht="24">
       <c r="A58" s="12"/>
       <c r="B58" s="19">
-        <v>10.199999999999999</v>
+        <v>9.6999999999999993</v>
       </c>
       <c r="C58" s="6"/>
       <c r="D58" s="6"/>
       <c r="E58" s="6" t="s">
-        <v>60</v>
-      </c>
-      <c r="F58" s="14" t="s">
-        <v>61</v>
+        <v>104</v>
+      </c>
+      <c r="F58" s="23" t="s">
+        <v>105</v>
       </c>
       <c r="G58" s="4"/>
       <c r="H58" s="4"/>
@@ -3659,37 +4027,35 @@
         <v>8</v>
       </c>
     </row>
-    <row r="59" spans="1:9" ht="24">
+    <row r="59" spans="1:9" ht="48">
       <c r="A59" s="12"/>
       <c r="B59" s="19">
-        <v>10.3</v>
-      </c>
-      <c r="C59" s="6"/>
-      <c r="D59" s="6"/>
-      <c r="E59" s="6" t="s">
-        <v>62</v>
-      </c>
-      <c r="F59" s="6" t="s">
-        <v>63</v>
-      </c>
+        <v>10</v>
+      </c>
+      <c r="C59" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="D59" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="E59" s="6"/>
+      <c r="F59" s="6"/>
       <c r="G59" s="4"/>
       <c r="H59" s="4"/>
-      <c r="I59" s="16" t="s">
-        <v>8</v>
-      </c>
+      <c r="I59" s="4"/>
     </row>
     <row r="60" spans="1:9" ht="24">
       <c r="A60" s="12"/>
       <c r="B60" s="19">
-        <v>10.4</v>
+        <v>10.1</v>
       </c>
       <c r="C60" s="6"/>
       <c r="D60" s="6"/>
       <c r="E60" s="6" t="s">
-        <v>64</v>
+        <v>51</v>
       </c>
       <c r="F60" s="6" t="s">
-        <v>65</v>
+        <v>52</v>
       </c>
       <c r="G60" s="4"/>
       <c r="H60" s="4"/>
@@ -3700,15 +4066,15 @@
     <row r="61" spans="1:9" ht="24">
       <c r="A61" s="12"/>
       <c r="B61" s="19">
-        <v>10.5</v>
+        <v>10.199999999999999</v>
       </c>
       <c r="C61" s="6"/>
       <c r="D61" s="6"/>
       <c r="E61" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="F61" s="6" t="s">
-        <v>18</v>
+        <v>58</v>
+      </c>
+      <c r="F61" s="14" t="s">
+        <v>59</v>
       </c>
       <c r="G61" s="4"/>
       <c r="H61" s="4"/>
@@ -3719,15 +4085,15 @@
     <row r="62" spans="1:9" ht="24">
       <c r="A62" s="12"/>
       <c r="B62" s="19">
-        <v>10.6</v>
+        <v>10.3</v>
       </c>
       <c r="C62" s="6"/>
       <c r="D62" s="6"/>
       <c r="E62" s="6" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="F62" s="6" t="s">
-        <v>73</v>
+        <v>61</v>
       </c>
       <c r="G62" s="4"/>
       <c r="H62" s="4"/>
@@ -3735,35 +4101,37 @@
         <v>8</v>
       </c>
     </row>
-    <row r="63" spans="1:9" ht="48">
+    <row r="63" spans="1:9" ht="24">
       <c r="A63" s="12"/>
       <c r="B63" s="19">
-        <v>11</v>
-      </c>
-      <c r="C63" s="9" t="s">
-        <v>45</v>
-      </c>
-      <c r="D63" s="10" t="s">
-        <v>47</v>
-      </c>
-      <c r="E63" s="6"/>
-      <c r="F63" s="6"/>
+        <v>10.4</v>
+      </c>
+      <c r="C63" s="6"/>
+      <c r="D63" s="6"/>
+      <c r="E63" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="F63" s="6" t="s">
+        <v>63</v>
+      </c>
       <c r="G63" s="4"/>
       <c r="H63" s="4"/>
-      <c r="I63" s="4"/>
+      <c r="I63" s="16" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="64" spans="1:9" ht="24">
       <c r="A64" s="12"/>
       <c r="B64" s="19">
-        <v>11.1</v>
+        <v>10.5</v>
       </c>
       <c r="C64" s="6"/>
       <c r="D64" s="6"/>
       <c r="E64" s="6" t="s">
-        <v>53</v>
+        <v>17</v>
       </c>
       <c r="F64" s="6" t="s">
-        <v>54</v>
+        <v>18</v>
       </c>
       <c r="G64" s="4"/>
       <c r="H64" s="4"/>
@@ -3774,15 +4142,15 @@
     <row r="65" spans="1:9" ht="24">
       <c r="A65" s="12"/>
       <c r="B65" s="19">
-        <v>11.2</v>
+        <v>10.6</v>
       </c>
       <c r="C65" s="6"/>
       <c r="D65" s="6"/>
       <c r="E65" s="6" t="s">
-        <v>60</v>
-      </c>
-      <c r="F65" s="14" t="s">
-        <v>61</v>
+        <v>64</v>
+      </c>
+      <c r="F65" s="6" t="s">
+        <v>71</v>
       </c>
       <c r="G65" s="4"/>
       <c r="H65" s="4"/>
@@ -3790,37 +4158,35 @@
         <v>8</v>
       </c>
     </row>
-    <row r="66" spans="1:9" ht="24">
+    <row r="66" spans="1:9" ht="48">
       <c r="A66" s="12"/>
       <c r="B66" s="19">
-        <v>11.3</v>
-      </c>
-      <c r="C66" s="6"/>
-      <c r="D66" s="6"/>
-      <c r="E66" s="6" t="s">
-        <v>62</v>
-      </c>
-      <c r="F66" s="6" t="s">
-        <v>63</v>
-      </c>
+        <v>11</v>
+      </c>
+      <c r="C66" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="D66" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="E66" s="6"/>
+      <c r="F66" s="6"/>
       <c r="G66" s="4"/>
       <c r="H66" s="4"/>
-      <c r="I66" s="16" t="s">
-        <v>8</v>
-      </c>
+      <c r="I66" s="4"/>
     </row>
     <row r="67" spans="1:9" ht="24">
       <c r="A67" s="12"/>
       <c r="B67" s="19">
-        <v>11.4</v>
+        <v>11.1</v>
       </c>
       <c r="C67" s="6"/>
       <c r="D67" s="6"/>
       <c r="E67" s="6" t="s">
-        <v>64</v>
+        <v>51</v>
       </c>
       <c r="F67" s="6" t="s">
-        <v>65</v>
+        <v>52</v>
       </c>
       <c r="G67" s="4"/>
       <c r="H67" s="4"/>
@@ -3831,15 +4197,15 @@
     <row r="68" spans="1:9" ht="24">
       <c r="A68" s="12"/>
       <c r="B68" s="19">
-        <v>11.5</v>
+        <v>11.2</v>
       </c>
       <c r="C68" s="6"/>
       <c r="D68" s="6"/>
       <c r="E68" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="F68" s="6" t="s">
-        <v>34</v>
+        <v>58</v>
+      </c>
+      <c r="F68" s="14" t="s">
+        <v>59</v>
       </c>
       <c r="G68" s="4"/>
       <c r="H68" s="4"/>
@@ -3850,15 +4216,15 @@
     <row r="69" spans="1:9" ht="24">
       <c r="A69" s="12"/>
       <c r="B69" s="19">
-        <v>11.6</v>
+        <v>11.3</v>
       </c>
       <c r="C69" s="6"/>
       <c r="D69" s="6"/>
       <c r="E69" s="6" t="s">
-        <v>74</v>
+        <v>60</v>
       </c>
       <c r="F69" s="6" t="s">
-        <v>73</v>
+        <v>61</v>
       </c>
       <c r="G69" s="4"/>
       <c r="H69" s="4"/>
@@ -3866,35 +4232,37 @@
         <v>8</v>
       </c>
     </row>
-    <row r="70" spans="1:9" ht="48">
+    <row r="70" spans="1:9" ht="24">
       <c r="A70" s="12"/>
       <c r="B70" s="19">
-        <v>12</v>
-      </c>
-      <c r="C70" s="9" t="s">
-        <v>45</v>
-      </c>
-      <c r="D70" s="10" t="s">
-        <v>32</v>
-      </c>
-      <c r="E70" s="6"/>
-      <c r="F70" s="6"/>
+        <v>11.4</v>
+      </c>
+      <c r="C70" s="6"/>
+      <c r="D70" s="6"/>
+      <c r="E70" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="F70" s="6" t="s">
+        <v>63</v>
+      </c>
       <c r="G70" s="4"/>
       <c r="H70" s="4"/>
-      <c r="I70" s="4"/>
+      <c r="I70" s="16" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="71" spans="1:9" ht="24">
       <c r="A71" s="12"/>
       <c r="B71" s="19">
-        <v>12.1</v>
-      </c>
-      <c r="C71" s="15"/>
-      <c r="D71" s="13"/>
+        <v>11.5</v>
+      </c>
+      <c r="C71" s="6"/>
+      <c r="D71" s="6"/>
       <c r="E71" s="6" t="s">
-        <v>53</v>
+        <v>32</v>
       </c>
       <c r="F71" s="6" t="s">
-        <v>54</v>
+        <v>33</v>
       </c>
       <c r="G71" s="4"/>
       <c r="H71" s="4"/>
@@ -3905,15 +4273,15 @@
     <row r="72" spans="1:9" ht="24">
       <c r="A72" s="12"/>
       <c r="B72" s="19">
-        <v>12.2</v>
-      </c>
-      <c r="C72" s="15"/>
-      <c r="D72" s="13"/>
+        <v>11.6</v>
+      </c>
+      <c r="C72" s="6"/>
+      <c r="D72" s="6"/>
       <c r="E72" s="6" t="s">
-        <v>60</v>
-      </c>
-      <c r="F72" s="14" t="s">
-        <v>61</v>
+        <v>72</v>
+      </c>
+      <c r="F72" s="6" t="s">
+        <v>71</v>
       </c>
       <c r="G72" s="4"/>
       <c r="H72" s="4"/>
@@ -3921,37 +4289,35 @@
         <v>8</v>
       </c>
     </row>
-    <row r="73" spans="1:9" ht="24">
+    <row r="73" spans="1:9" ht="48">
       <c r="A73" s="12"/>
       <c r="B73" s="19">
-        <v>12.3</v>
-      </c>
-      <c r="C73" s="15"/>
-      <c r="D73" s="13"/>
-      <c r="E73" s="6" t="s">
-        <v>62</v>
-      </c>
-      <c r="F73" s="6" t="s">
-        <v>63</v>
-      </c>
+        <v>12</v>
+      </c>
+      <c r="C73" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="D73" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="E73" s="6"/>
+      <c r="F73" s="6"/>
       <c r="G73" s="4"/>
       <c r="H73" s="4"/>
-      <c r="I73" s="16" t="s">
-        <v>8</v>
-      </c>
+      <c r="I73" s="4"/>
     </row>
     <row r="74" spans="1:9" ht="24">
       <c r="A74" s="12"/>
       <c r="B74" s="19">
-        <v>12.4</v>
+        <v>12.1</v>
       </c>
       <c r="C74" s="15"/>
       <c r="D74" s="13"/>
       <c r="E74" s="6" t="s">
-        <v>64</v>
+        <v>51</v>
       </c>
       <c r="F74" s="6" t="s">
-        <v>65</v>
+        <v>52</v>
       </c>
       <c r="G74" s="4"/>
       <c r="H74" s="4"/>
@@ -3962,15 +4328,15 @@
     <row r="75" spans="1:9" ht="24">
       <c r="A75" s="12"/>
       <c r="B75" s="19">
-        <v>12.5</v>
-      </c>
-      <c r="C75" s="6"/>
-      <c r="D75" s="6"/>
+        <v>12.2</v>
+      </c>
+      <c r="C75" s="15"/>
+      <c r="D75" s="13"/>
       <c r="E75" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="F75" s="6" t="s">
-        <v>19</v>
+        <v>58</v>
+      </c>
+      <c r="F75" s="14" t="s">
+        <v>59</v>
       </c>
       <c r="G75" s="4"/>
       <c r="H75" s="4"/>
@@ -3978,113 +4344,113 @@
         <v>8</v>
       </c>
     </row>
-    <row r="76" spans="1:9" ht="48">
+    <row r="76" spans="1:9" ht="24">
       <c r="A76" s="12"/>
       <c r="B76" s="19">
-        <v>12.6</v>
-      </c>
-      <c r="C76" s="6"/>
-      <c r="D76" s="6"/>
+        <v>12.3</v>
+      </c>
+      <c r="C76" s="15"/>
+      <c r="D76" s="13"/>
       <c r="E76" s="6" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="F76" s="6" t="s">
-        <v>81</v>
-      </c>
-      <c r="G76" s="6" t="s">
-        <v>83</v>
-      </c>
+        <v>61</v>
+      </c>
+      <c r="G76" s="4"/>
       <c r="H76" s="4"/>
-      <c r="I76" s="11" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="77" spans="1:9" ht="48">
+      <c r="I76" s="16" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="77" spans="1:9" ht="24">
       <c r="A77" s="12"/>
       <c r="B77" s="19">
-        <v>13</v>
-      </c>
-      <c r="C77" s="9" t="s">
-        <v>45</v>
-      </c>
-      <c r="D77" s="10" t="s">
-        <v>35</v>
-      </c>
-      <c r="E77" s="6"/>
-      <c r="F77" s="6"/>
-      <c r="G77" s="6"/>
+        <v>12.4</v>
+      </c>
+      <c r="C77" s="15"/>
+      <c r="D77" s="13"/>
+      <c r="E77" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="F77" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="G77" s="4"/>
       <c r="H77" s="4"/>
-      <c r="I77" s="11"/>
+      <c r="I77" s="16" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="78" spans="1:9" ht="24">
       <c r="A78" s="12"/>
       <c r="B78" s="19">
-        <v>13.1</v>
+        <v>12.5</v>
       </c>
       <c r="C78" s="6"/>
       <c r="D78" s="6"/>
       <c r="E78" s="6" t="s">
-        <v>79</v>
+        <v>24</v>
       </c>
       <c r="F78" s="6" t="s">
-        <v>54</v>
-      </c>
-      <c r="G78" s="6"/>
+        <v>19</v>
+      </c>
+      <c r="G78" s="4"/>
       <c r="H78" s="4"/>
       <c r="I78" s="16" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="79" spans="1:9" ht="24">
+    <row r="79" spans="1:9" ht="48">
       <c r="A79" s="12"/>
       <c r="B79" s="19">
-        <v>13.2</v>
+        <v>12.6</v>
       </c>
       <c r="C79" s="6"/>
       <c r="D79" s="6"/>
       <c r="E79" s="6" t="s">
-        <v>80</v>
-      </c>
-      <c r="F79" s="14" t="s">
-        <v>61</v>
-      </c>
-      <c r="G79" s="6"/>
+        <v>64</v>
+      </c>
+      <c r="F79" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="G79" s="6" t="s">
+        <v>81</v>
+      </c>
       <c r="H79" s="4"/>
-      <c r="I79" s="16" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="80" spans="1:9" ht="24">
+      <c r="I79" s="11" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="80" spans="1:9" ht="48">
       <c r="A80" s="12"/>
       <c r="B80" s="19">
-        <v>13.3</v>
-      </c>
-      <c r="C80" s="6"/>
-      <c r="D80" s="6"/>
-      <c r="E80" s="6" t="s">
-        <v>62</v>
-      </c>
-      <c r="F80" s="6" t="s">
-        <v>63</v>
-      </c>
+        <v>13</v>
+      </c>
+      <c r="C80" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="D80" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="E80" s="6"/>
+      <c r="F80" s="6"/>
       <c r="G80" s="6"/>
       <c r="H80" s="4"/>
-      <c r="I80" s="16" t="s">
-        <v>8</v>
-      </c>
+      <c r="I80" s="11"/>
     </row>
     <row r="81" spans="1:9" ht="24">
       <c r="A81" s="12"/>
       <c r="B81" s="19">
-        <v>13.4</v>
+        <v>13.1</v>
       </c>
       <c r="C81" s="6"/>
       <c r="D81" s="6"/>
       <c r="E81" s="6" t="s">
-        <v>64</v>
+        <v>77</v>
       </c>
       <c r="F81" s="6" t="s">
-        <v>65</v>
+        <v>52</v>
       </c>
       <c r="G81" s="6"/>
       <c r="H81" s="4"/>
@@ -4095,72 +4461,72 @@
     <row r="82" spans="1:9" ht="24">
       <c r="A82" s="12"/>
       <c r="B82" s="19">
-        <v>13.5</v>
+        <v>13.2</v>
       </c>
       <c r="C82" s="6"/>
       <c r="D82" s="6"/>
       <c r="E82" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="F82" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="G82" s="4"/>
+        <v>78</v>
+      </c>
+      <c r="F82" s="14" t="s">
+        <v>59</v>
+      </c>
+      <c r="G82" s="6"/>
       <c r="H82" s="4"/>
       <c r="I82" s="16" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="83" spans="1:9" ht="48">
+    <row r="83" spans="1:9" ht="24">
       <c r="A83" s="12"/>
       <c r="B83" s="19">
-        <v>13.6</v>
+        <v>13.3</v>
       </c>
       <c r="C83" s="6"/>
       <c r="D83" s="6"/>
       <c r="E83" s="6" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="F83" s="6" t="s">
-        <v>82</v>
-      </c>
-      <c r="G83" s="6" t="s">
-        <v>20</v>
-      </c>
+        <v>61</v>
+      </c>
+      <c r="G83" s="6"/>
       <c r="H83" s="4"/>
-      <c r="I83" s="11" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="84" spans="1:9" ht="48">
+      <c r="I83" s="16" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="84" spans="1:9" ht="24">
       <c r="A84" s="12"/>
       <c r="B84" s="19">
-        <v>14</v>
-      </c>
-      <c r="C84" s="9" t="s">
-        <v>44</v>
-      </c>
-      <c r="D84" s="10" t="s">
-        <v>92</v>
-      </c>
-      <c r="E84" s="6"/>
-      <c r="F84" s="6"/>
-      <c r="G84" s="4"/>
+        <v>13.4</v>
+      </c>
+      <c r="C84" s="6"/>
+      <c r="D84" s="6"/>
+      <c r="E84" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="F84" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="G84" s="6"/>
       <c r="H84" s="4"/>
-      <c r="I84" s="4"/>
+      <c r="I84" s="16" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="85" spans="1:9" ht="24">
       <c r="A85" s="12"/>
       <c r="B85" s="19">
-        <v>14.1</v>
-      </c>
-      <c r="C85" s="15"/>
-      <c r="D85" s="13"/>
+        <v>13.5</v>
+      </c>
+      <c r="C85" s="6"/>
+      <c r="D85" s="6"/>
       <c r="E85" s="6" t="s">
-        <v>53</v>
+        <v>25</v>
       </c>
       <c r="F85" s="6" t="s">
-        <v>54</v>
+        <v>19</v>
       </c>
       <c r="G85" s="4"/>
       <c r="H85" s="4"/>
@@ -4168,56 +4534,56 @@
         <v>8</v>
       </c>
     </row>
-    <row r="86" spans="1:9" ht="24">
+    <row r="86" spans="1:9" ht="48">
       <c r="A86" s="12"/>
       <c r="B86" s="19">
-        <v>14.2</v>
+        <v>13.6</v>
       </c>
       <c r="C86" s="6"/>
       <c r="D86" s="6"/>
       <c r="E86" s="6" t="s">
-        <v>84</v>
+        <v>64</v>
       </c>
       <c r="F86" s="6" t="s">
-        <v>85</v>
-      </c>
-      <c r="G86" s="4"/>
+        <v>80</v>
+      </c>
+      <c r="G86" s="6" t="s">
+        <v>20</v>
+      </c>
       <c r="H86" s="4"/>
-      <c r="I86" s="16" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="87" spans="1:9" ht="24">
+      <c r="I86" s="11" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="87" spans="1:9" ht="48">
       <c r="A87" s="12"/>
       <c r="B87" s="19">
-        <v>14.3</v>
-      </c>
-      <c r="C87" s="6"/>
-      <c r="D87" s="6"/>
-      <c r="E87" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="F87" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C87" s="9" t="s">
         <v>42</v>
       </c>
+      <c r="D87" s="10" t="s">
+        <v>90</v>
+      </c>
+      <c r="E87" s="6"/>
+      <c r="F87" s="6"/>
       <c r="G87" s="4"/>
       <c r="H87" s="4"/>
-      <c r="I87" s="16" t="s">
-        <v>8</v>
-      </c>
+      <c r="I87" s="4"/>
     </row>
     <row r="88" spans="1:9" ht="24">
       <c r="A88" s="12"/>
       <c r="B88" s="19">
-        <v>14.4</v>
-      </c>
-      <c r="C88" s="6"/>
-      <c r="D88" s="6"/>
+        <v>14.1</v>
+      </c>
+      <c r="C88" s="15"/>
+      <c r="D88" s="13"/>
       <c r="E88" s="6" t="s">
-        <v>21</v>
+        <v>51</v>
       </c>
       <c r="F88" s="6" t="s">
-        <v>22</v>
+        <v>52</v>
       </c>
       <c r="G88" s="4"/>
       <c r="H88" s="4"/>
@@ -4228,15 +4594,15 @@
     <row r="89" spans="1:9" ht="24">
       <c r="A89" s="12"/>
       <c r="B89" s="19">
-        <v>14.5</v>
+        <v>14.2</v>
       </c>
       <c r="C89" s="6"/>
       <c r="D89" s="6"/>
       <c r="E89" s="6" t="s">
-        <v>62</v>
+        <v>82</v>
       </c>
       <c r="F89" s="6" t="s">
-        <v>63</v>
+        <v>83</v>
       </c>
       <c r="G89" s="4"/>
       <c r="H89" s="4"/>
@@ -4247,15 +4613,15 @@
     <row r="90" spans="1:9" ht="24">
       <c r="A90" s="12"/>
       <c r="B90" s="19">
-        <v>14.6</v>
+        <v>14.3</v>
       </c>
       <c r="C90" s="6"/>
       <c r="D90" s="6"/>
       <c r="E90" s="6" t="s">
-        <v>86</v>
+        <v>112</v>
       </c>
       <c r="F90" s="6" t="s">
-        <v>65</v>
+        <v>113</v>
       </c>
       <c r="G90" s="4"/>
       <c r="H90" s="4"/>
@@ -4263,18 +4629,18 @@
         <v>8</v>
       </c>
     </row>
-    <row r="91" spans="1:9" ht="36">
+    <row r="91" spans="1:9" ht="24">
       <c r="A91" s="12"/>
       <c r="B91" s="19">
-        <v>14.7</v>
+        <v>14.4</v>
       </c>
       <c r="C91" s="6"/>
       <c r="D91" s="6"/>
       <c r="E91" s="6" t="s">
-        <v>66</v>
+        <v>111</v>
       </c>
       <c r="F91" s="6" t="s">
-        <v>87</v>
+        <v>22</v>
       </c>
       <c r="G91" s="4"/>
       <c r="H91" s="4"/>
@@ -4282,180 +4648,198 @@
         <v>8</v>
       </c>
     </row>
-    <row r="92" spans="1:9" ht="48">
+    <row r="92" spans="1:9" ht="24">
       <c r="A92" s="12"/>
       <c r="B92" s="19">
-        <v>15</v>
-      </c>
-      <c r="C92" s="9" t="s">
-        <v>44</v>
-      </c>
-      <c r="D92" s="10" t="s">
-        <v>93</v>
-      </c>
-      <c r="E92" s="6"/>
-      <c r="F92" s="6"/>
+        <v>14.5</v>
+      </c>
+      <c r="C92" s="6"/>
+      <c r="D92" s="6"/>
+      <c r="E92" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="F92" s="6" t="s">
+        <v>61</v>
+      </c>
       <c r="G92" s="4"/>
       <c r="H92" s="4"/>
-      <c r="I92" s="16"/>
+      <c r="I92" s="16" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="93" spans="1:9" ht="24">
       <c r="A93" s="12"/>
       <c r="B93" s="19">
-        <v>15.1</v>
+        <v>14.6</v>
       </c>
       <c r="C93" s="6"/>
       <c r="D93" s="6"/>
       <c r="E93" s="6" t="s">
-        <v>53</v>
+        <v>84</v>
       </c>
       <c r="F93" s="6" t="s">
-        <v>54</v>
+        <v>63</v>
       </c>
       <c r="G93" s="4"/>
       <c r="H93" s="4"/>
-      <c r="I93" s="16"/>
-    </row>
-    <row r="94" spans="1:9" ht="24">
+      <c r="I93" s="16" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="94" spans="1:9" ht="36">
       <c r="A94" s="12"/>
       <c r="B94" s="19">
-        <v>15.2</v>
+        <v>14.7</v>
       </c>
       <c r="C94" s="6"/>
       <c r="D94" s="6"/>
       <c r="E94" s="6" t="s">
-        <v>84</v>
+        <v>64</v>
       </c>
       <c r="F94" s="6" t="s">
         <v>85</v>
       </c>
       <c r="G94" s="4"/>
       <c r="H94" s="4"/>
-      <c r="I94" s="16"/>
-    </row>
-    <row r="95" spans="1:9" ht="36">
+      <c r="I94" s="16" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="95" spans="1:9" ht="24">
       <c r="A95" s="12"/>
       <c r="B95" s="19">
-        <v>15.3</v>
+        <v>14.8</v>
       </c>
       <c r="C95" s="6"/>
       <c r="D95" s="6"/>
       <c r="E95" s="6" t="s">
-        <v>94</v>
-      </c>
-      <c r="F95" s="6" t="s">
-        <v>42</v>
+        <v>104</v>
+      </c>
+      <c r="F95" s="23" t="s">
+        <v>107</v>
       </c>
       <c r="G95" s="4"/>
       <c r="H95" s="4"/>
-      <c r="I95" s="16"/>
-    </row>
-    <row r="96" spans="1:9" ht="24">
+      <c r="I95" s="16" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="96" spans="1:9" ht="48">
       <c r="A96" s="12"/>
       <c r="B96" s="19">
-        <v>15.4</v>
-      </c>
-      <c r="C96" s="6"/>
-      <c r="D96" s="6"/>
-      <c r="E96" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="F96" s="6" t="s">
-        <v>95</v>
-      </c>
+        <v>15</v>
+      </c>
+      <c r="C96" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="D96" s="10" t="s">
+        <v>91</v>
+      </c>
+      <c r="E96" s="6"/>
+      <c r="F96" s="6"/>
       <c r="G96" s="4"/>
       <c r="H96" s="4"/>
-      <c r="I96" s="16"/>
+      <c r="I96" s="4"/>
     </row>
     <row r="97" spans="1:9" ht="24">
       <c r="A97" s="12"/>
       <c r="B97" s="19">
-        <v>15.5</v>
+        <v>15.1</v>
       </c>
       <c r="C97" s="6"/>
       <c r="D97" s="6"/>
       <c r="E97" s="6" t="s">
-        <v>62</v>
+        <v>51</v>
       </c>
       <c r="F97" s="6" t="s">
-        <v>63</v>
+        <v>52</v>
       </c>
       <c r="G97" s="4"/>
       <c r="H97" s="4"/>
-      <c r="I97" s="16"/>
+      <c r="I97" s="16" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="98" spans="1:9" ht="24">
       <c r="A98" s="12"/>
       <c r="B98" s="19">
-        <v>15.6</v>
+        <v>15.2</v>
       </c>
       <c r="C98" s="6"/>
       <c r="D98" s="6"/>
       <c r="E98" s="6" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="F98" s="6" t="s">
-        <v>65</v>
+        <v>83</v>
       </c>
       <c r="G98" s="4"/>
       <c r="H98" s="4"/>
-      <c r="I98" s="16"/>
+      <c r="I98" s="16" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="99" spans="1:9" ht="36">
       <c r="A99" s="12"/>
       <c r="B99" s="19">
-        <v>15.7</v>
+        <v>15.3</v>
       </c>
       <c r="C99" s="6"/>
       <c r="D99" s="6"/>
       <c r="E99" s="6" t="s">
-        <v>66</v>
+        <v>109</v>
       </c>
       <c r="F99" s="6" t="s">
-        <v>96</v>
+        <v>110</v>
       </c>
       <c r="G99" s="4"/>
       <c r="H99" s="4"/>
-      <c r="I99" s="16"/>
-    </row>
-    <row r="100" spans="1:9" ht="48">
+      <c r="I99" s="16" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="100" spans="1:9" ht="24">
       <c r="A100" s="12"/>
       <c r="B100" s="19">
-        <v>16</v>
-      </c>
-      <c r="C100" s="9" t="s">
-        <v>44</v>
-      </c>
-      <c r="D100" s="10" t="s">
-        <v>98</v>
-      </c>
-      <c r="E100" s="6"/>
-      <c r="F100" s="6"/>
+        <v>15.4</v>
+      </c>
+      <c r="C100" s="6"/>
+      <c r="D100" s="6"/>
+      <c r="E100" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="F100" s="6" t="s">
+        <v>92</v>
+      </c>
       <c r="G100" s="4"/>
       <c r="H100" s="4"/>
-      <c r="I100" s="16"/>
+      <c r="I100" s="16" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="101" spans="1:9" ht="24">
       <c r="A101" s="12"/>
       <c r="B101" s="19">
-        <v>16.100000000000001</v>
+        <v>15.5</v>
       </c>
       <c r="C101" s="6"/>
       <c r="D101" s="6"/>
       <c r="E101" s="6" t="s">
-        <v>53</v>
+        <v>60</v>
       </c>
       <c r="F101" s="6" t="s">
-        <v>54</v>
+        <v>61</v>
       </c>
       <c r="G101" s="4"/>
       <c r="H101" s="4"/>
-      <c r="I101" s="16"/>
+      <c r="I101" s="16" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="102" spans="1:9" ht="24">
       <c r="A102" s="12"/>
       <c r="B102" s="19">
-        <v>16.2</v>
+        <v>15.6</v>
       </c>
       <c r="C102" s="6"/>
       <c r="D102" s="6"/>
@@ -4463,92 +4847,100 @@
         <v>84</v>
       </c>
       <c r="F102" s="6" t="s">
-        <v>85</v>
+        <v>63</v>
       </c>
       <c r="G102" s="4"/>
       <c r="H102" s="4"/>
-      <c r="I102" s="16"/>
+      <c r="I102" s="16" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="103" spans="1:9" ht="36">
       <c r="A103" s="12"/>
       <c r="B103" s="19">
-        <v>16.3</v>
+        <v>15.7</v>
       </c>
       <c r="C103" s="6"/>
       <c r="D103" s="6"/>
       <c r="E103" s="6" t="s">
-        <v>94</v>
+        <v>64</v>
       </c>
       <c r="F103" s="6" t="s">
-        <v>42</v>
+        <v>93</v>
       </c>
       <c r="G103" s="4"/>
       <c r="H103" s="4"/>
-      <c r="I103" s="16"/>
+      <c r="I103" s="16" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="104" spans="1:9" ht="24">
       <c r="A104" s="12"/>
       <c r="B104" s="19">
-        <v>16.399999999999999</v>
+        <v>15.8</v>
       </c>
       <c r="C104" s="6"/>
       <c r="D104" s="6"/>
       <c r="E104" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="F104" s="6" t="s">
-        <v>95</v>
+        <v>104</v>
+      </c>
+      <c r="F104" s="23" t="s">
+        <v>107</v>
       </c>
       <c r="G104" s="4"/>
       <c r="H104" s="4"/>
-      <c r="I104" s="16"/>
-    </row>
-    <row r="105" spans="1:9" ht="24">
+      <c r="I104" s="16" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="105" spans="1:9" ht="48">
       <c r="A105" s="12"/>
       <c r="B105" s="19">
-        <v>16.5</v>
-      </c>
-      <c r="C105" s="6"/>
-      <c r="D105" s="6"/>
-      <c r="E105" s="6" t="s">
-        <v>106</v>
-      </c>
-      <c r="F105" s="6" t="s">
-        <v>97</v>
-      </c>
+        <v>16</v>
+      </c>
+      <c r="C105" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="D105" s="10" t="s">
+        <v>108</v>
+      </c>
+      <c r="E105" s="6"/>
+      <c r="F105" s="6"/>
       <c r="G105" s="4"/>
       <c r="H105" s="4"/>
-      <c r="I105" s="16"/>
-    </row>
-    <row r="106" spans="1:9" ht="48">
+      <c r="I105" s="4"/>
+    </row>
+    <row r="106" spans="1:9" ht="24">
       <c r="A106" s="12"/>
       <c r="B106" s="19">
-        <v>17</v>
-      </c>
-      <c r="C106" s="9" t="s">
-        <v>45</v>
-      </c>
-      <c r="D106" s="10" t="s">
-        <v>36</v>
-      </c>
-      <c r="E106" s="6"/>
-      <c r="F106" s="6"/>
+        <v>16.100000000000001</v>
+      </c>
+      <c r="C106" s="6"/>
+      <c r="D106" s="6"/>
+      <c r="E106" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="F106" s="6" t="s">
+        <v>52</v>
+      </c>
       <c r="G106" s="4"/>
       <c r="H106" s="4"/>
-      <c r="I106" s="4"/>
+      <c r="I106" s="16" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="107" spans="1:9" ht="24">
       <c r="A107" s="12"/>
       <c r="B107" s="19">
-        <v>17.100000000000001</v>
-      </c>
-      <c r="C107" s="15"/>
-      <c r="D107" s="13"/>
-      <c r="E107" s="14" t="s">
-        <v>41</v>
-      </c>
-      <c r="F107" s="17" t="s">
-        <v>52</v>
+        <v>16.2</v>
+      </c>
+      <c r="C107" s="6"/>
+      <c r="D107" s="6"/>
+      <c r="E107" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="F107" s="6" t="s">
+        <v>83</v>
       </c>
       <c r="G107" s="4"/>
       <c r="H107" s="4"/>
@@ -4556,18 +4948,18 @@
         <v>8</v>
       </c>
     </row>
-    <row r="108" spans="1:9" ht="24">
+    <row r="108" spans="1:9" ht="36">
       <c r="A108" s="12"/>
       <c r="B108" s="19">
-        <v>17.2</v>
-      </c>
-      <c r="C108" s="15"/>
-      <c r="D108" s="13"/>
-      <c r="E108" s="14" t="s">
-        <v>88</v>
-      </c>
-      <c r="F108" s="17" t="s">
-        <v>89</v>
+        <v>16.3</v>
+      </c>
+      <c r="C108" s="6"/>
+      <c r="D108" s="6"/>
+      <c r="E108" s="6" t="s">
+        <v>109</v>
+      </c>
+      <c r="F108" s="6" t="s">
+        <v>110</v>
       </c>
       <c r="G108" s="4"/>
       <c r="H108" s="4"/>
@@ -4578,15 +4970,15 @@
     <row r="109" spans="1:9" ht="24">
       <c r="A109" s="12"/>
       <c r="B109" s="19">
-        <v>17.3</v>
+        <v>16.399999999999999</v>
       </c>
       <c r="C109" s="6"/>
       <c r="D109" s="6"/>
-      <c r="E109" s="14" t="s">
-        <v>90</v>
-      </c>
-      <c r="F109" s="14" t="s">
-        <v>91</v>
+      <c r="E109" s="6" t="s">
+        <v>111</v>
+      </c>
+      <c r="F109" s="6" t="s">
+        <v>92</v>
       </c>
       <c r="G109" s="4"/>
       <c r="H109" s="4"/>
@@ -4597,15 +4989,15 @@
     <row r="110" spans="1:9" ht="24">
       <c r="A110" s="12"/>
       <c r="B110" s="19">
-        <v>17.399999999999999</v>
+        <v>16.5</v>
       </c>
       <c r="C110" s="6"/>
       <c r="D110" s="6"/>
-      <c r="E110" s="14" t="s">
-        <v>37</v>
-      </c>
-      <c r="F110" s="14" t="s">
-        <v>23</v>
+      <c r="E110" s="6" t="s">
+        <v>102</v>
+      </c>
+      <c r="F110" s="6" t="s">
+        <v>94</v>
       </c>
       <c r="G110" s="4"/>
       <c r="H110" s="4"/>
@@ -4613,19 +5005,19 @@
         <v>8</v>
       </c>
     </row>
-    <row r="111" spans="1:9" ht="24">
+    <row r="111" spans="1:9" ht="48">
       <c r="A111" s="12"/>
       <c r="B111" s="19">
-        <v>17.5</v>
-      </c>
-      <c r="C111" s="6"/>
-      <c r="D111" s="6"/>
-      <c r="E111" s="6" t="s">
-        <v>99</v>
-      </c>
-      <c r="F111" s="14" t="s">
-        <v>101</v>
-      </c>
+        <v>17</v>
+      </c>
+      <c r="C111" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="D111" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="E111" s="6"/>
+      <c r="F111" s="6"/>
       <c r="G111" s="4"/>
       <c r="H111" s="4"/>
       <c r="I111" s="4"/>
@@ -4633,109 +5025,171 @@
     <row r="112" spans="1:9" ht="24">
       <c r="A112" s="12"/>
       <c r="B112" s="19">
-        <v>17.600000000000001</v>
-      </c>
-      <c r="C112" s="6"/>
-      <c r="D112" s="6"/>
-      <c r="E112" s="6" t="s">
-        <v>100</v>
-      </c>
-      <c r="F112" s="6" t="s">
-        <v>102</v>
+        <v>17.100000000000001</v>
+      </c>
+      <c r="C112" s="15"/>
+      <c r="D112" s="13"/>
+      <c r="E112" s="14" t="s">
+        <v>40</v>
+      </c>
+      <c r="F112" s="17" t="s">
+        <v>50</v>
       </c>
       <c r="G112" s="4"/>
       <c r="H112" s="4"/>
-      <c r="I112" s="4"/>
-    </row>
-    <row r="113" spans="1:9">
+      <c r="I112" s="16" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="113" spans="1:9" ht="24">
       <c r="A113" s="12"/>
-      <c r="B113" s="20"/>
-      <c r="C113" s="6"/>
-      <c r="D113" s="6"/>
-      <c r="E113" s="6"/>
-      <c r="F113" s="6"/>
+      <c r="B113" s="19">
+        <v>17.2</v>
+      </c>
+      <c r="C113" s="15"/>
+      <c r="D113" s="13"/>
+      <c r="E113" s="14" t="s">
+        <v>86</v>
+      </c>
+      <c r="F113" s="17" t="s">
+        <v>87</v>
+      </c>
       <c r="G113" s="4"/>
       <c r="H113" s="4"/>
-      <c r="I113" s="4"/>
-    </row>
-    <row r="114" spans="1:9">
+      <c r="I113" s="16" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="114" spans="1:9" ht="24">
       <c r="A114" s="12"/>
-      <c r="B114" s="20"/>
+      <c r="B114" s="19">
+        <v>17.3</v>
+      </c>
       <c r="C114" s="6"/>
       <c r="D114" s="6"/>
-      <c r="E114" s="6"/>
-      <c r="F114" s="6"/>
+      <c r="E114" s="14" t="s">
+        <v>88</v>
+      </c>
+      <c r="F114" s="14" t="s">
+        <v>89</v>
+      </c>
       <c r="G114" s="4"/>
       <c r="H114" s="4"/>
-      <c r="I114" s="4"/>
-    </row>
-    <row r="115" spans="1:9">
+      <c r="I114" s="16" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="115" spans="1:9" ht="24">
       <c r="A115" s="12"/>
-      <c r="B115" s="20"/>
+      <c r="B115" s="19">
+        <v>17.399999999999999</v>
+      </c>
       <c r="C115" s="6"/>
       <c r="D115" s="6"/>
-      <c r="E115" s="6"/>
-      <c r="F115" s="6"/>
+      <c r="E115" s="14" t="s">
+        <v>36</v>
+      </c>
+      <c r="F115" s="14" t="s">
+        <v>23</v>
+      </c>
       <c r="G115" s="4"/>
       <c r="H115" s="4"/>
-      <c r="I115" s="4"/>
-    </row>
-    <row r="116" spans="1:9">
+      <c r="I115" s="16" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="116" spans="1:9" ht="24">
       <c r="A116" s="12"/>
-      <c r="B116" s="20"/>
+      <c r="B116" s="19">
+        <v>17.5</v>
+      </c>
       <c r="C116" s="6"/>
       <c r="D116" s="6"/>
-      <c r="E116" s="6"/>
-      <c r="F116" s="6"/>
+      <c r="E116" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="F116" s="14" t="s">
+        <v>97</v>
+      </c>
       <c r="G116" s="4"/>
       <c r="H116" s="4"/>
-      <c r="I116" s="4"/>
-    </row>
-    <row r="117" spans="1:9">
+      <c r="I116" s="16" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="117" spans="1:9" ht="24">
       <c r="A117" s="12"/>
-      <c r="B117" s="20"/>
+      <c r="B117" s="19">
+        <v>17.600000000000001</v>
+      </c>
       <c r="C117" s="6"/>
       <c r="D117" s="6"/>
-      <c r="E117" s="6"/>
-      <c r="F117" s="6"/>
+      <c r="E117" s="6" t="s">
+        <v>96</v>
+      </c>
+      <c r="F117" s="6" t="s">
+        <v>98</v>
+      </c>
       <c r="G117" s="4"/>
       <c r="H117" s="4"/>
-      <c r="I117" s="4"/>
+      <c r="I117" s="16" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="118" spans="1:9">
-      <c r="A118" s="2"/>
-      <c r="C118" s="3"/>
-      <c r="D118" s="3"/>
-      <c r="E118" s="3"/>
-      <c r="F118" s="3"/>
+      <c r="A118" s="12"/>
+      <c r="B118" s="20"/>
+      <c r="C118" s="6"/>
+      <c r="D118" s="6"/>
+      <c r="E118" s="6"/>
+      <c r="F118" s="6"/>
+      <c r="G118" s="4"/>
+      <c r="H118" s="4"/>
+      <c r="I118" s="4"/>
     </row>
     <row r="119" spans="1:9">
-      <c r="A119" s="2"/>
-      <c r="C119" s="3"/>
-      <c r="D119" s="3"/>
-      <c r="E119" s="3"/>
-      <c r="F119" s="3"/>
+      <c r="A119" s="12"/>
+      <c r="B119" s="20"/>
+      <c r="C119" s="6"/>
+      <c r="D119" s="6"/>
+      <c r="E119" s="6"/>
+      <c r="F119" s="6"/>
+      <c r="G119" s="4"/>
+      <c r="H119" s="4"/>
+      <c r="I119" s="4"/>
     </row>
     <row r="120" spans="1:9">
-      <c r="A120" s="2"/>
-      <c r="C120" s="3"/>
-      <c r="D120" s="3"/>
-      <c r="E120" s="3"/>
-      <c r="F120" s="3"/>
+      <c r="A120" s="12"/>
+      <c r="B120" s="20"/>
+      <c r="C120" s="6"/>
+      <c r="D120" s="6"/>
+      <c r="E120" s="6"/>
+      <c r="F120" s="6"/>
+      <c r="G120" s="4"/>
+      <c r="H120" s="4"/>
+      <c r="I120" s="4"/>
     </row>
     <row r="121" spans="1:9">
-      <c r="A121" s="2"/>
-      <c r="C121" s="3"/>
-      <c r="D121" s="3"/>
-      <c r="E121" s="3"/>
-      <c r="F121" s="3"/>
+      <c r="A121" s="12"/>
+      <c r="B121" s="20"/>
+      <c r="C121" s="6"/>
+      <c r="D121" s="6"/>
+      <c r="E121" s="6"/>
+      <c r="F121" s="6"/>
+      <c r="G121" s="4"/>
+      <c r="H121" s="4"/>
+      <c r="I121" s="4"/>
     </row>
     <row r="122" spans="1:9">
-      <c r="A122" s="2"/>
-      <c r="C122" s="3"/>
-      <c r="D122" s="3"/>
-      <c r="E122" s="3"/>
-      <c r="F122" s="3"/>
+      <c r="A122" s="12"/>
+      <c r="B122" s="20"/>
+      <c r="C122" s="6"/>
+      <c r="D122" s="6"/>
+      <c r="E122" s="6"/>
+      <c r="F122" s="6"/>
+      <c r="G122" s="4"/>
+      <c r="H122" s="4"/>
+      <c r="I122" s="4"/>
     </row>
     <row r="123" spans="1:9">
       <c r="A123" s="2"/>
@@ -8685,80 +9139,140 @@
       <c r="E686" s="3"/>
       <c r="F686" s="3"/>
     </row>
+    <row r="687" spans="1:6">
+      <c r="A687" s="2"/>
+      <c r="C687" s="3"/>
+      <c r="D687" s="3"/>
+      <c r="E687" s="3"/>
+      <c r="F687" s="3"/>
+    </row>
+    <row r="688" spans="1:6">
+      <c r="A688" s="2"/>
+      <c r="C688" s="3"/>
+      <c r="D688" s="3"/>
+      <c r="E688" s="3"/>
+      <c r="F688" s="3"/>
+    </row>
+    <row r="689" spans="1:6">
+      <c r="A689" s="2"/>
+      <c r="C689" s="3"/>
+      <c r="D689" s="3"/>
+      <c r="E689" s="3"/>
+      <c r="F689" s="3"/>
+    </row>
+    <row r="690" spans="1:6">
+      <c r="A690" s="2"/>
+      <c r="C690" s="3"/>
+      <c r="D690" s="3"/>
+      <c r="E690" s="3"/>
+      <c r="F690" s="3"/>
+    </row>
+    <row r="691" spans="1:6">
+      <c r="A691" s="2"/>
+      <c r="C691" s="3"/>
+      <c r="D691" s="3"/>
+      <c r="E691" s="3"/>
+      <c r="F691" s="3"/>
+    </row>
   </sheetData>
   <conditionalFormatting sqref="I27:I30 I6:I14">
-    <cfRule type="containsText" dxfId="14" priority="12" operator="containsText" text="Passed">
+    <cfRule type="containsText" dxfId="19" priority="17" operator="containsText" text="Passed">
       <formula>NOT(ISERROR(SEARCH(("Passed"),(I6))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I27:I30 I6:I14">
-    <cfRule type="containsText" dxfId="13" priority="13" operator="containsText" text="Failed">
+    <cfRule type="containsText" dxfId="18" priority="18" operator="containsText" text="Failed">
       <formula>NOT(ISERROR(SEARCH(("Failed"),(I6))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I27:I30 I6:I14">
-    <cfRule type="containsText" dxfId="12" priority="14" operator="containsText" text="Blocked">
+    <cfRule type="containsText" dxfId="17" priority="19" operator="containsText" text="Blocked">
       <formula>NOT(ISERROR(SEARCH(("Blocked"),(I6))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I27:I30 I6:I14">
-    <cfRule type="containsText" dxfId="11" priority="15" operator="containsText" text="✓">
+    <cfRule type="containsText" dxfId="16" priority="20" operator="containsText" text="✓">
       <formula>NOT(ISERROR(SEARCH(("✓"),(I6))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I27:I30 I6:I14">
-    <cfRule type="containsText" dxfId="10" priority="16" operator="containsText" text="✗">
+    <cfRule type="containsText" dxfId="15" priority="21" operator="containsText" text="✗">
       <formula>NOT(ISERROR(SEARCH(("✗"),(I6))))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I76">
-    <cfRule type="containsText" dxfId="9" priority="6" operator="containsText" text="Passed">
-      <formula>NOT(ISERROR(SEARCH(("Passed"),(I76))))</formula>
+  <conditionalFormatting sqref="I79">
+    <cfRule type="containsText" dxfId="14" priority="11" operator="containsText" text="Passed">
+      <formula>NOT(ISERROR(SEARCH(("Passed"),(I79))))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I76">
-    <cfRule type="containsText" dxfId="8" priority="7" operator="containsText" text="Failed">
-      <formula>NOT(ISERROR(SEARCH(("Failed"),(I76))))</formula>
+  <conditionalFormatting sqref="I79">
+    <cfRule type="containsText" dxfId="13" priority="12" operator="containsText" text="Failed">
+      <formula>NOT(ISERROR(SEARCH(("Failed"),(I79))))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I76">
-    <cfRule type="containsText" dxfId="7" priority="8" operator="containsText" text="Blocked">
-      <formula>NOT(ISERROR(SEARCH(("Blocked"),(I76))))</formula>
+  <conditionalFormatting sqref="I79">
+    <cfRule type="containsText" dxfId="12" priority="13" operator="containsText" text="Blocked">
+      <formula>NOT(ISERROR(SEARCH(("Blocked"),(I79))))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I76">
-    <cfRule type="containsText" dxfId="6" priority="9" operator="containsText" text="✓">
-      <formula>NOT(ISERROR(SEARCH(("✓"),(I76))))</formula>
+  <conditionalFormatting sqref="I79">
+    <cfRule type="containsText" dxfId="11" priority="14" operator="containsText" text="✓">
+      <formula>NOT(ISERROR(SEARCH(("✓"),(I79))))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I76">
-    <cfRule type="containsText" dxfId="5" priority="10" operator="containsText" text="✗">
-      <formula>NOT(ISERROR(SEARCH(("✗"),(I76))))</formula>
+  <conditionalFormatting sqref="I79">
+    <cfRule type="containsText" dxfId="10" priority="15" operator="containsText" text="✗">
+      <formula>NOT(ISERROR(SEARCH(("✗"),(I79))))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I83">
-    <cfRule type="containsText" dxfId="4" priority="1" operator="containsText" text="Passed">
-      <formula>NOT(ISERROR(SEARCH(("Passed"),(I83))))</formula>
+  <conditionalFormatting sqref="I86">
+    <cfRule type="containsText" dxfId="9" priority="6" operator="containsText" text="Passed">
+      <formula>NOT(ISERROR(SEARCH(("Passed"),(I86))))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I83">
-    <cfRule type="containsText" dxfId="3" priority="2" operator="containsText" text="Failed">
-      <formula>NOT(ISERROR(SEARCH(("Failed"),(I83))))</formula>
+  <conditionalFormatting sqref="I86">
+    <cfRule type="containsText" dxfId="8" priority="7" operator="containsText" text="Failed">
+      <formula>NOT(ISERROR(SEARCH(("Failed"),(I86))))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I83">
-    <cfRule type="containsText" dxfId="2" priority="3" operator="containsText" text="Blocked">
-      <formula>NOT(ISERROR(SEARCH(("Blocked"),(I83))))</formula>
+  <conditionalFormatting sqref="I86">
+    <cfRule type="containsText" dxfId="7" priority="8" operator="containsText" text="Blocked">
+      <formula>NOT(ISERROR(SEARCH(("Blocked"),(I86))))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I83">
-    <cfRule type="containsText" dxfId="1" priority="4" operator="containsText" text="✓">
-      <formula>NOT(ISERROR(SEARCH(("✓"),(I83))))</formula>
+  <conditionalFormatting sqref="I86">
+    <cfRule type="containsText" dxfId="6" priority="9" operator="containsText" text="✓">
+      <formula>NOT(ISERROR(SEARCH(("✓"),(I86))))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I83">
+  <conditionalFormatting sqref="I86">
+    <cfRule type="containsText" dxfId="5" priority="10" operator="containsText" text="✗">
+      <formula>NOT(ISERROR(SEARCH(("✗"),(I86))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I16:I19">
+    <cfRule type="containsText" dxfId="4" priority="1" operator="containsText" text="Passed">
+      <formula>NOT(ISERROR(SEARCH(("Passed"),(I16))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I16:I19">
+    <cfRule type="containsText" dxfId="3" priority="2" operator="containsText" text="Failed">
+      <formula>NOT(ISERROR(SEARCH(("Failed"),(I16))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I16:I19">
+    <cfRule type="containsText" dxfId="2" priority="3" operator="containsText" text="Blocked">
+      <formula>NOT(ISERROR(SEARCH(("Blocked"),(I16))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I16:I19">
+    <cfRule type="containsText" dxfId="1" priority="4" operator="containsText" text="✓">
+      <formula>NOT(ISERROR(SEARCH(("✓"),(I16))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I16:I19">
     <cfRule type="containsText" dxfId="0" priority="5" operator="containsText" text="✗">
-      <formula>NOT(ISERROR(SEARCH(("✗"),(I83))))</formula>
+      <formula>NOT(ISERROR(SEARCH(("✗"),(I16))))</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>